<commit_message>
version order multi shop
</commit_message>
<xml_diff>
--- a/DataTest/AddProduct.xlsx
+++ b/DataTest/AddProduct.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ThuyDung\DATN_Selenium_Java_ThuyDung\DataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuceedu-my.sharepoint.com/personal/dung47265_huce_edu_vn/Documents/DATN_47265/DATN_Selenium_Java_ThuyDung1/DATN_Selenium_Java_ThuyDung/DataTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_C7709F7FC38686363B104D63CAF3B37F46C3C10A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB2BD660-F807-423E-BE7B-38C3C3DD889D}"/>
   <bookViews>
-    <workbookView xWindow="11124" yWindow="2652" windowWidth="11916" windowHeight="8880" tabRatio="602"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddProduct" sheetId="1" r:id="rId1"/>
@@ -78,9 +79,6 @@
     <t>gio-qua-1.jpg</t>
   </si>
   <si>
-    <t>Cake</t>
-  </si>
-  <si>
     <t>01-03-2024 00:00:00 to 31-05-2024 00:00:00</t>
   </si>
   <si>
@@ -103,12 +101,15 @@
   </si>
   <si>
     <t>unit null</t>
+  </si>
+  <si>
+    <t>Sweet Cake</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -426,30 +427,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="46" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.6640625" style="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" ht="37.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,15 +485,15 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="54">
+    <row r="2" spans="1:12" ht="75">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -507,7 +508,7 @@
         <v>138000</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="1">
         <v>999</v>
@@ -522,15 +523,15 @@
         <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="54">
+    <row r="3" spans="1:12" ht="75">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
@@ -545,13 +546,13 @@
         <v>500000</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1">
         <v>300</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" s="1">
         <v>2</v>
@@ -560,15 +561,15 @@
         <v>18</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="54">
+    <row r="4" spans="1:12" ht="75">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1">
         <v>1500</v>
@@ -580,13 +581,13 @@
         <v>500000</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1">
         <v>300</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" s="1">
         <v>2</v>
@@ -595,7 +596,7 @@
         <v>18</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version add product - tax
</commit_message>
<xml_diff>
--- a/DataTest/AddProduct.xlsx
+++ b/DataTest/AddProduct.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuceedu-my.sharepoint.com/personal/dung47265_huce_edu_vn/Documents/DATN_47265/DATN_Selenium_Java_ThuyDung1/DATN_Selenium_Java_ThuyDung/DataTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_C7709F7FC38686363B104D63CAF3B37F46C3C10A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB2BD660-F807-423E-BE7B-38C3C3DD889D}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{39367BAC-AE9B-4ADC-8C25-966DD0CD35FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87DD6FFF-63D3-401B-B7A9-2F3EA2964259}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>productName</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>Sweet Cake</t>
+  </si>
+  <si>
+    <t>vat</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75"/>
@@ -450,7 +453,7 @@
     <col min="12" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="37.5">
+    <row r="1" spans="1:13" ht="37.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,8 +490,11 @@
       <c r="L1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="75">
+    <row r="2" spans="1:13" ht="75">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -525,8 +531,11 @@
       <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="M2" s="1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="75">
+    <row r="3" spans="1:13" ht="75">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -563,8 +572,11 @@
       <c r="L3" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="M3" s="1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" ht="75">
+    <row r="4" spans="1:13" ht="75">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -597,6 +609,9 @@
       </c>
       <c r="L4" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="M4" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version check cart test with product variant
</commit_message>
<xml_diff>
--- a/DataTest/AddProduct.xlsx
+++ b/DataTest/AddProduct.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nuceedu-my.sharepoint.com/personal/dung47265_huce_edu_vn/Documents/DATN_47265/DATN_Selenium_Java_ThuyDung1/DATN_Selenium_Java_ThuyDung/DataTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{39367BAC-AE9B-4ADC-8C25-966DD0CD35FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87DD6FFF-63D3-401B-B7A9-2F3EA2964259}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{39367BAC-AE9B-4ADC-8C25-966DD0CD35FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA3D6ABA-7920-42CB-91F0-5FD72C26B8FD}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75"/>
@@ -532,7 +532,7 @@
         <v>24</v>
       </c>
       <c r="M2" s="1">
-        <v>5</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="75">
@@ -573,7 +573,7 @@
         <v>25</v>
       </c>
       <c r="M3" s="1">
-        <v>2</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="75">
@@ -611,7 +611,7 @@
         <v>26</v>
       </c>
       <c r="M4" s="1">
-        <v>2</v>
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
version update edit product
</commit_message>
<xml_diff>
--- a/DataTest/AddProduct.xlsx
+++ b/DataTest/AddProduct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VTTDung\OneDrive - HUCE\DATN_47265\DATN_Selenium_Java_ThuyDung1\DATN_Selenium_Java_ThuyDung\DataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13ABDD15-C820-4C50-8452-6F301B02A40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAA322A-521D-4337-83BF-6E2B3C45D626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="2925" windowWidth="22905" windowHeight="11295" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="1560" windowWidth="22905" windowHeight="11295" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddProduct" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>productName</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>vat</t>
+  </si>
+  <si>
+    <t>gio-qua-2.jpg</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="B1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75"/>
@@ -585,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M4" s="1">
         <v>3000</v>

</xml_diff>